<commit_message>
Update schedule with TRR schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/specky/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352A6D8E-360E-1C43-98CE-EEA08C42357A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD9CC1B-0ADD-6041-8A16-2D3F8EA6E484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$J$32</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$J$30</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>date</t>
   </si>
@@ -103,129 +103,9 @@
     <t>link_room</t>
   </si>
   <si>
-    <t>topics/linux/slide_linux_intro.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/qYp8shSMJ-0</t>
-  </si>
-  <si>
-    <t>topics/linux/lab_linux_intro.html</t>
-  </si>
-  <si>
     <t>Lunch</t>
   </si>
   <si>
-    <t>topics/uppmax/intro/slide_uppmax_intro.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/cxEtfKN91q4</t>
-  </si>
-  <si>
-    <t>topics/uppmax/intro/lab_uppmax_intro.html</t>
-  </si>
-  <si>
-    <t>File types in Bioinformatics</t>
-  </si>
-  <si>
-    <t>topics/linux/slide_linux_filetypes.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/7MR1qUZQ94w</t>
-  </si>
-  <si>
-    <t>topics/linux/lab_linux_filetypes.html</t>
-  </si>
-  <si>
-    <t>Better terminal experience</t>
-  </si>
-  <si>
-    <t>topics/linux/slide_qol_termexp.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/RGbONVWOaDo</t>
-  </si>
-  <si>
-    <t>Quality control</t>
-  </si>
-  <si>
-    <t>topics/other/slide_qc.pdf</t>
-  </si>
-  <si>
-    <t>topics/other/lab_qc.html</t>
-  </si>
-  <si>
-    <t>https://youtu.be/gytTBNSWpFc</t>
-  </si>
-  <si>
-    <t>Advanced Bash</t>
-  </si>
-  <si>
-    <t>topics/linux/slide_linux_advanced.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/n3IpUHIodM8</t>
-  </si>
-  <si>
-    <t>topics/linux/lab_linux_advanced.html</t>
-  </si>
-  <si>
-    <t>NGS tech &amp; challenges</t>
-  </si>
-  <si>
-    <t>topics/other/slide_sequencing.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/5sUzkrucL1E</t>
-  </si>
-  <si>
-    <t>Variant-calling workflow</t>
-  </si>
-  <si>
-    <t>topics/vc/slide_vc.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/NxRECdxKP40</t>
-  </si>
-  <si>
-    <t>topics/vc/lab_vc.html</t>
-  </si>
-  <si>
-    <t>GATK best practices</t>
-  </si>
-  <si>
-    <t>https://youtu.be/-cL0CI07-Es</t>
-  </si>
-  <si>
-    <t>RNA-Seq workflow</t>
-  </si>
-  <si>
-    <t>topics/rnaseq/slide_rnaseq.html</t>
-  </si>
-  <si>
-    <t>https://youtu.be/gC_nslHgSa8</t>
-  </si>
-  <si>
-    <t>topics/rnaseq/lab_rnaseq.html</t>
-  </si>
-  <si>
-    <t>Data management practices</t>
-  </si>
-  <si>
-    <t>topics/other/slide_data_management.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/PfcrDlhY1zE</t>
-  </si>
-  <si>
-    <t>NBIS</t>
-  </si>
-  <si>
-    <t>topics/other/slide_nbis.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/4HbSAEU5iBM</t>
-  </si>
-  <si>
     <t>25/11/2024</t>
   </si>
   <si>
@@ -241,9 +121,6 @@
     <t>29/11/2024</t>
   </si>
   <si>
-    <t>Course Dinner</t>
-  </si>
-  <si>
     <t>Setting up and troubleshooting installations</t>
   </si>
   <si>
@@ -275,6 +152,90 @@
   </si>
   <si>
     <t>Stockholm</t>
+  </si>
+  <si>
+    <t>lectures/git/git.html</t>
+  </si>
+  <si>
+    <t>… continued: Snakemake</t>
+  </si>
+  <si>
+    <t>Organise your analyses using workflow managers: Snakemake</t>
+  </si>
+  <si>
+    <t>Organise your analyses using workflow managers: Nextflow</t>
+  </si>
+  <si>
+    <t>Wrap-up day 2</t>
+  </si>
+  <si>
+    <t>Course dinner</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Grappa+Matsal+%26+Bar/@59.3406761,18.0349875,17z/data=!3m1!4b1!4m6!3m5!1s0x465f9d7a3ac32e91:0x9b6cd7aea9744f09!8m2!3d59.3406761!4d18.0375624!16s%2Fg%2F1tftpqfg?entry=ttu&amp;g_ep=EgoyMDI0MDkzMC4wIKXMDSoASAFQAw%3D%3D</t>
+  </si>
+  <si>
+    <t>… continued: Nextflow</t>
+  </si>
+  <si>
+    <t>Writing computational notebooks and reproducible reports: Quarto</t>
+  </si>
+  <si>
+    <t>… continued: Quarto</t>
+  </si>
+  <si>
+    <t>Writing computational notebooks and reproducible reports: Jupyter</t>
+  </si>
+  <si>
+    <t>Wrap-up day 3</t>
+  </si>
+  <si>
+    <t>… continued: Jupyter</t>
+  </si>
+  <si>
+    <t>Working with containers</t>
+  </si>
+  <si>
+    <t>… continued: Containers</t>
+  </si>
+  <si>
+    <t>Wrap-up day 4</t>
+  </si>
+  <si>
+    <t>Putting it all together</t>
+  </si>
+  <si>
+    <t>continued: Putting it all together</t>
+  </si>
+  <si>
+    <t>Final wrap-up and end of the course</t>
+  </si>
+  <si>
+    <t>lectures/conda/git.html</t>
+  </si>
+  <si>
+    <t>lectures/data-management/data-management.html</t>
+  </si>
+  <si>
+    <t>lectures/introduction/introduction.html</t>
+  </si>
+  <si>
+    <t>lectures/snakemake/snakemake.html</t>
+  </si>
+  <si>
+    <t>lectures/nextflow/nextflow.html</t>
+  </si>
+  <si>
+    <t>lectures/quarto/quarto.html</t>
+  </si>
+  <si>
+    <t>lectures/jupyter/jupyter.html</t>
+  </si>
+  <si>
+    <t>lectures/containers/containers.html</t>
+  </si>
+  <si>
+    <t>lectures/putting-it-together/putting-it-together.html</t>
   </si>
 </sst>
 </file>
@@ -741,22 +702,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="10.6640625" style="1"/>
@@ -796,17 +757,17 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -815,17 +776,15 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
@@ -833,10 +792,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -845,10 +801,13 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -857,17 +816,15 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
@@ -875,10 +832,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -887,7 +841,7 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -896,7 +850,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -905,10 +859,13 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -917,55 +874,50 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="3">
         <v>0.375</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="3">
-        <v>0.39583333333333298</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" s="3">
-        <v>0.45833333333333298</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -974,246 +926,362 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="C17" s="3">
-        <v>0.58333333333333304</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C18" s="3">
         <v>0.625</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C19" s="3">
-        <v>0.375</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C20" s="3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C21" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.375</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
-        <v>0.58333333333333304</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
-        <v>0.375</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C24" s="3">
-        <v>0.39583333333333298</v>
+        <v>0.5</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C25" s="3">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C26" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C27" s="3">
-        <v>0.58333333333333304</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C28" s="3">
-        <v>0.75</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C29" s="3">
-        <v>0.375</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C30" s="3">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.40625</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C32" s="3">
-        <v>0.58333333333333304</v>
+        <v>0.4375</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C33" s="3">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C34" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C36" s="3">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="3">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C38" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C40" s="3">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="3">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C43" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C44" s="3">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C45" s="3">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C46" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="I12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="I14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="I16" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="I17" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="I19" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="I21" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="I23" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="I26" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="I31" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="I32" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId13"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix schedule missing content
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD9CC1B-0ADD-6041-8A16-2D3F8EA6E484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AF6207-374C-0545-AA3E-0AEBF1D30876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$J$30</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$30</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -172,9 +172,6 @@
     <t>Course dinner</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/Grappa+Matsal+%26+Bar/@59.3406761,18.0349875,17z/data=!3m1!4b1!4m6!3m5!1s0x465f9d7a3ac32e91:0x9b6cd7aea9744f09!8m2!3d59.3406761!4d18.0375624!16s%2Fg%2F1tftpqfg?entry=ttu&amp;g_ep=EgoyMDI0MDkzMC4wIKXMDSoASAFQAw%3D%3D</t>
-  </si>
-  <si>
     <t>… continued: Nextflow</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>lectures/putting-it-together/putting-it-together.html</t>
+  </si>
+  <si>
+    <t>assistant</t>
   </si>
 </sst>
 </file>
@@ -702,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,14 +716,15 @@
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="5" width="57.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.6640625" style="1"/>
+    <col min="7" max="7" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,19 +744,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -770,7 +774,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -781,12 +785,12 @@
       <c r="F3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
         <v>0.43402777777777773</v>
       </c>
@@ -795,7 +799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
         <v>0.44444444444444442</v>
       </c>
@@ -806,11 +810,11 @@
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C6" s="3">
         <v>0.46527777777777773</v>
       </c>
@@ -821,12 +825,12 @@
       <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
         <v>0.5</v>
       </c>
@@ -835,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C8" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -844,7 +848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
         <v>0.61111111111111105</v>
       </c>
@@ -853,7 +857,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
         <v>0.625</v>
       </c>
@@ -864,11 +868,11 @@
       <c r="F10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C11" s="3">
         <v>0.69791666666666663</v>
       </c>
@@ -880,7 +884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -897,12 +901,12 @@
       <c r="F12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C13" s="3">
         <v>0.43055555555555558</v>
       </c>
@@ -911,7 +915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C14" s="3">
         <v>0.44444444444444442</v>
       </c>
@@ -920,7 +924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" s="3">
         <v>0.5</v>
       </c>
@@ -928,9 +932,9 @@
       <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -948,7 +952,8 @@
         <v>18</v>
       </c>
       <c r="F17" s="5"/>
-      <c r="I17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C18" s="3">
@@ -961,8 +966,8 @@
       <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>50</v>
+      <c r="H18" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -976,7 +981,7 @@
       <c r="F19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C20" s="3">
@@ -986,10 +991,7 @@
       <c r="E20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -1003,7 +1005,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1014,7 +1016,7 @@
       <c r="E22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
@@ -1022,7 +1024,7 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1033,7 +1035,7 @@
       <c r="E24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C25" s="3">
@@ -1041,13 +1043,13 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>51</v>
+      <c r="H25" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1065,7 +1067,7 @@
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1074,13 +1076,13 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>52</v>
+      <c r="H28" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1089,7 +1091,7 @@
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>24</v>
@@ -1107,9 +1109,9 @@
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31" s="3">
@@ -1117,13 +1119,13 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>53</v>
+      <c r="H31" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1135,16 +1137,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C33" s="3">
         <v>0.4513888888888889</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C34" s="3">
         <v>0.5</v>
       </c>
@@ -1153,16 +1155,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C35" s="3">
         <v>0.54166666666666663</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C36" s="3">
         <v>0.59722222222222221</v>
       </c>
@@ -1171,28 +1173,28 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C37" s="3">
         <v>0.61111111111111105</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C38" s="3">
         <v>0.69791666666666663</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -1204,16 +1206,16 @@
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C40" s="3">
         <v>0.43055555555555558</v>
       </c>
@@ -1222,16 +1224,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C41" s="3">
         <v>0.44444444444444442</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C42" s="3">
         <v>0.5</v>
       </c>
@@ -1240,16 +1242,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C43" s="3">
         <v>0.54166666666666663</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C44" s="3">
         <v>0.59722222222222221</v>
       </c>
@@ -1258,22 +1260,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C45" s="3">
         <v>0.61111111111111105</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C46" s="3">
         <v>0.65625</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Changed start_time and end_time to time
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-reproducible-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AF6207-374C-0545-AA3E-0AEBF1D30876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69AAC5A-F7E6-3E4C-9FD8-2662B0ED74E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$30</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$J$30</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>date</t>
   </si>
@@ -79,12 +79,6 @@
     <t>room</t>
   </si>
   <si>
-    <t>start_time</t>
-  </si>
-  <si>
-    <t>end_time</t>
-  </si>
-  <si>
     <t>topic</t>
   </si>
   <si>
@@ -236,6 +230,9 @@
   </si>
   <si>
     <t>assistant</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -702,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,18 +710,17 @@
     <col min="1" max="1" width="10.6640625" style="1"/>
     <col min="2" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.6640625" style="1"/>
+    <col min="4" max="4" width="57.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,553 +728,505 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
         <v>0.43402777777777773</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="3">
         <v>0.46527777777777773</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
         <v>0.5</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
         <v>0.61111111111111105</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
         <v>0.625</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" s="3">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="3">
         <v>0.375</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="3">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" s="3">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="3">
         <v>0.5</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C17" s="3">
         <v>0.61111111111111105</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C18" s="3">
         <v>0.625</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C19" s="3">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C20" s="3">
         <v>0.75</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="3">
         <v>0.375</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D21" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C24" s="3">
         <v>0.5</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C25" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C26" s="3">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C27" s="3">
         <v>0.61805555555555558</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C28" s="3">
         <v>0.63888888888888895</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C29" s="3">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="E29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C30" s="3">
         <v>0.375</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C31" s="3">
         <v>0.40625</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C32" s="3">
         <v>0.4375</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D32" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C33" s="3">
         <v>0.4513888888888889</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C34" s="3">
         <v>0.5</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C35" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C36" s="3">
         <v>0.59722222222222221</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D36" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C37" s="3">
         <v>0.61111111111111105</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D37" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C38" s="3">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="E38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C39" s="3">
         <v>0.375</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C40" s="3">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D40" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C41" s="3">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D41" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C42" s="3">
         <v>0.5</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C43" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D43" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C44" s="3">
         <v>0.59722222222222221</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D44" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C45" s="3">
         <v>0.61111111111111105</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D45" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C46" s="3">
         <v>0.65625</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="E46" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tutorial links to schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-reproducible-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69AAC5A-F7E6-3E4C-9FD8-2662B0ED74E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F571FB-F3F3-B549-8E7E-C1B3241FD226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>date</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Putting it all together</t>
   </si>
   <si>
-    <t>continued: Putting it all together</t>
-  </si>
-  <si>
     <t>Final wrap-up and end of the course</t>
   </si>
   <si>
@@ -233,6 +230,30 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>… continued: Putting it all together</t>
+  </si>
+  <si>
+    <t>pages/git.html</t>
+  </si>
+  <si>
+    <t>pages/conda.html</t>
+  </si>
+  <si>
+    <t>pages/snakemake.html</t>
+  </si>
+  <si>
+    <t>pages/nextflow.html</t>
+  </si>
+  <si>
+    <t>pages/quarto.html</t>
+  </si>
+  <si>
+    <t>pages/jupyter.html</t>
+  </si>
+  <si>
+    <t>pages/containers.html</t>
   </si>
 </sst>
 </file>
@@ -702,7 +723,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +735,7 @@
     <col min="5" max="5" width="30" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.6640625" style="1"/>
@@ -728,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -737,7 +758,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -777,7 +798,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -800,7 +821,7 @@
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -816,6 +837,9 @@
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -833,6 +857,9 @@
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
@@ -853,7 +880,10 @@
         <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -884,7 +914,10 @@
         <v>23</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -903,6 +936,9 @@
       <c r="D14" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H14" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="3">
@@ -920,6 +956,9 @@
       <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H16" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C17" s="3">
@@ -943,7 +982,10 @@
         <v>22</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -980,6 +1022,9 @@
       <c r="D21" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="H21" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
@@ -997,6 +1042,9 @@
       <c r="D23" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="H23" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C24" s="3">
@@ -1018,7 +1066,10 @@
         <v>22</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1036,6 +1087,9 @@
       <c r="D27" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="H27" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C28" s="3">
@@ -1048,7 +1102,10 @@
         <v>23</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1075,6 +1132,9 @@
       <c r="D30" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="H30" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1088,7 +1148,10 @@
         <v>23</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1099,15 +1162,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C33" s="3">
         <v>0.4513888888888889</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C34" s="3">
         <v>0.5</v>
       </c>
@@ -1115,15 +1181,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C35" s="3">
         <v>0.54166666666666663</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C36" s="3">
         <v>0.59722222222222221</v>
       </c>
@@ -1131,15 +1200,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C37" s="3">
         <v>0.61111111111111105</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C38" s="3">
         <v>0.69791666666666663</v>
       </c>
@@ -1150,7 +1222,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
@@ -1167,10 +1239,10 @@
         <v>22</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C40" s="3">
         <v>0.43055555555555558</v>
       </c>
@@ -1178,15 +1250,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C41" s="3">
         <v>0.44444444444444442</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C42" s="3">
         <v>0.5</v>
       </c>
@@ -1194,15 +1266,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C43" s="3">
         <v>0.54166666666666663</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C44" s="3">
         <v>0.59722222222222221</v>
       </c>
@@ -1210,20 +1282,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C45" s="3">
         <v>0.61111111111111105</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C46" s="3">
         <v>0.65625</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
conda session title aligned with resources
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -133,7 +133,7 @@
     <t xml:space="preserve">… continued: Git</t>
   </si>
   <si>
-    <t xml:space="preserve">Mastering your environment with Conda</t>
+    <t xml:space="preserve">Controlling your environment with Conda</t>
   </si>
   <si>
     <t xml:space="preserve">lectures/conda/conda.html</t>
@@ -635,7 +635,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -722,7 +722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="3" t="n">
         <v>0.444444444444444</v>
       </c>

</xml_diff>

<commit_message>
Add missing introduction link in schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C74F37-60FD-714B-B232-4E36D4D64528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26420" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="schedule" vbProcedure="false">Sheet1!$A$1:$J$30</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$J$30</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -23,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Unknown Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +52,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">To link to a room map, add under link_room</t>
+          <t>To link to a room map, add under link_room</t>
         </r>
       </text>
     </comment>
@@ -56,200 +61,202 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">topic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instructor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link_slide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link_lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link_youtube</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link_room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stockholm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setting up and troubleshooting installations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Reproducible Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erik Fasterius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/introduction/introduction.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Break</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data management and project organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Sundh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/data-management/data-management.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version tracking and distributing your code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/git/git.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages/git.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lunch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… continued: Git</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controlling your environment with Conda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/conda/conda.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages/conda.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrap-up day 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organise your analyses using workflow managers: Snakemake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/snakemake/snakemake.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages/snakemake.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… continued: Snakemake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organise your analyses using workflow managers: Nextflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/nextflow/nextflow.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages/nextflow.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrap-up day 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Course dinner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… continued: Nextflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Writing computational notebooks and reproducible reports: Quarto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/quarto/quarto.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages/quarto.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… continued: Quarto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Writing computational notebooks and reproducible reports: Jupyter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/jupyter/jupyter.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages/jupyter.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrap-up day 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… continued: Jupyter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Working with containers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/containers/containers.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages/containers.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… continued: Containers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrap-up day 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Putting it all together</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lectures/putting-it-together/putting-it-together.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… continued: Putting it all together</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final wrap-up and end of the course</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>instructor</t>
+  </si>
+  <si>
+    <t>assistant</t>
+  </si>
+  <si>
+    <t>link_slide</t>
+  </si>
+  <si>
+    <t>link_lab</t>
+  </si>
+  <si>
+    <t>link_youtube</t>
+  </si>
+  <si>
+    <t>link_room</t>
+  </si>
+  <si>
+    <t>25/11/2024</t>
+  </si>
+  <si>
+    <t>Stockholm</t>
+  </si>
+  <si>
+    <t>Setting up and troubleshooting installations</t>
+  </si>
+  <si>
+    <t>Introduction to Reproducible Research</t>
+  </si>
+  <si>
+    <t>Erik Fasterius</t>
+  </si>
+  <si>
+    <t>lectures/introduction/introduction.html</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Data management and project organisation</t>
+  </si>
+  <si>
+    <t>John Sundh</t>
+  </si>
+  <si>
+    <t>lectures/data-management/data-management.html</t>
+  </si>
+  <si>
+    <t>Version tracking and distributing your code</t>
+  </si>
+  <si>
+    <t>lectures/git/git.html</t>
+  </si>
+  <si>
+    <t>pages/git.html</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>… continued: Git</t>
+  </si>
+  <si>
+    <t>Controlling your environment with Conda</t>
+  </si>
+  <si>
+    <t>lectures/conda/conda.html</t>
+  </si>
+  <si>
+    <t>pages/conda.html</t>
+  </si>
+  <si>
+    <t>Wrap-up day 1</t>
+  </si>
+  <si>
+    <t>26/11/2024</t>
+  </si>
+  <si>
+    <t>Organise your analyses using workflow managers: Snakemake</t>
+  </si>
+  <si>
+    <t>lectures/snakemake/snakemake.html</t>
+  </si>
+  <si>
+    <t>pages/snakemake.html</t>
+  </si>
+  <si>
+    <t>… continued: Snakemake</t>
+  </si>
+  <si>
+    <t>Organise your analyses using workflow managers: Nextflow</t>
+  </si>
+  <si>
+    <t>lectures/nextflow/nextflow.html</t>
+  </si>
+  <si>
+    <t>pages/nextflow.html</t>
+  </si>
+  <si>
+    <t>Wrap-up day 2</t>
+  </si>
+  <si>
+    <t>Course dinner</t>
+  </si>
+  <si>
+    <t>27/11/2024</t>
+  </si>
+  <si>
+    <t>… continued: Nextflow</t>
+  </si>
+  <si>
+    <t>Writing computational notebooks and reproducible reports: Quarto</t>
+  </si>
+  <si>
+    <t>lectures/quarto/quarto.html</t>
+  </si>
+  <si>
+    <t>pages/quarto.html</t>
+  </si>
+  <si>
+    <t>… continued: Quarto</t>
+  </si>
+  <si>
+    <t>Writing computational notebooks and reproducible reports: Jupyter</t>
+  </si>
+  <si>
+    <t>lectures/jupyter/jupyter.html</t>
+  </si>
+  <si>
+    <t>pages/jupyter.html</t>
+  </si>
+  <si>
+    <t>Wrap-up day 3</t>
+  </si>
+  <si>
+    <t>28/11/2024</t>
+  </si>
+  <si>
+    <t>… continued: Jupyter</t>
+  </si>
+  <si>
+    <t>Working with containers</t>
+  </si>
+  <si>
+    <t>lectures/containers/containers.html</t>
+  </si>
+  <si>
+    <t>pages/containers.html</t>
+  </si>
+  <si>
+    <t>… continued: Containers</t>
+  </si>
+  <si>
+    <t>Wrap-up day 4</t>
+  </si>
+  <si>
+    <t>29/11/2024</t>
+  </si>
+  <si>
+    <t>Putting it all together</t>
+  </si>
+  <si>
+    <t>lectures/putting-it-together/putting-it-together.html</t>
+  </si>
+  <si>
+    <t>… continued: Putting it all together</t>
+  </si>
+  <si>
+    <t>Final wrap-up and end of the course</t>
+  </si>
+  <si>
+    <t>pages/introduction.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="h:mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -258,28 +265,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -287,7 +279,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -321,7 +313,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -329,69 +321,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -450,60 +397,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -535,7 +498,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -559,7 +522,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -619,41 +582,40 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="57.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="45.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="10.66"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,23 +647,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="3">
         <v>0.375</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="3" t="n">
-        <v>0.416666666666667</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="3">
+        <v>0.41666666666666702</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -712,19 +674,22 @@
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="3" t="n">
-        <v>0.434027777777778</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="3">
+        <v>0.43402777777777801</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="3" t="n">
-        <v>0.444444444444444</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C5" s="3">
+        <v>0.44444444444444398</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -736,9 +701,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="3" t="n">
-        <v>0.465277777777778</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="3">
+        <v>0.46527777777777801</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>20</v>
@@ -754,17 +719,17 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="3" t="n">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7" s="3">
         <v>0.5</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="3" t="n">
-        <v>0.541666666666667</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="3">
+        <v>0.54166666666666696</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>24</v>
@@ -773,16 +738,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="3" t="n">
-        <v>0.611111111111111</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
+        <v>0.61111111111111105</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="3" t="n">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="3">
         <v>0.625</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -798,9 +763,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="3" t="n">
-        <v>0.697916666666667</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="3">
+        <v>0.69791666666666696</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>28</v>
@@ -809,14 +774,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="3">
         <v>0.375</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -833,17 +798,17 @@
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="3" t="n">
-        <v>0.430555555555556</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="3">
+        <v>0.43055555555555602</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="3" t="n">
-        <v>0.444444444444444</v>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="3">
+        <v>0.44444444444444398</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>33</v>
@@ -852,8 +817,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="3" t="n">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C15" s="3">
         <v>0.5</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -861,9 +826,9 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="3" t="n">
-        <v>0.541666666666667</v>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C16" s="3">
+        <v>0.54166666666666696</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>33</v>
@@ -872,9 +837,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="3" t="n">
-        <v>0.611111111111111</v>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="C17" s="3">
+        <v>0.61111111111111105</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -883,8 +848,8 @@
       <c r="F17" s="5"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="3" t="n">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C18" s="3">
         <v>0.625</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -900,9 +865,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="3" t="n">
-        <v>0.697916666666667</v>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="3">
+        <v>0.69791666666666696</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>37</v>
@@ -912,8 +877,8 @@
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="3" t="n">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C20" s="3">
         <v>0.75</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -921,14 +886,14 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="3">
         <v>0.375</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -938,18 +903,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="3" t="n">
-        <v>0.430555555555556</v>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C22" s="3">
+        <v>0.43055555555555602</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="3" t="n">
-        <v>0.444444444444444</v>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C23" s="3">
+        <v>0.44444444444444398</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -958,8 +923,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="3" t="n">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C24" s="3">
         <v>0.5</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -967,9 +932,9 @@
       </c>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="3" t="n">
-        <v>0.541666666666667</v>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C25" s="3">
+        <v>0.54166666666666696</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>41</v>
@@ -984,17 +949,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="3" t="n">
-        <v>0.604166666666667</v>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="3">
+        <v>0.60416666666666696</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="3" t="n">
-        <v>0.618055555555556</v>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="3">
+        <v>0.61805555555555602</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>44</v>
@@ -1003,9 +968,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="3" t="n">
-        <v>0.638888888888889</v>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="3">
+        <v>0.63888888888888895</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>45</v>
@@ -1020,9 +985,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="3" t="n">
-        <v>0.697916666666667</v>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C29" s="3">
+        <v>0.69791666666666696</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>48</v>
@@ -1031,14 +996,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="3">
         <v>0.375</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1049,8 +1014,8 @@
       </c>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="3" t="n">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C31" s="3">
         <v>0.40625</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1066,17 +1031,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="3" t="n">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C32" s="3">
         <v>0.4375</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="3" t="n">
-        <v>0.451388888888889</v>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C33" s="3">
+        <v>0.45138888888888901</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>54</v>
@@ -1085,17 +1050,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="3" t="n">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C34" s="3">
         <v>0.5</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="3" t="n">
-        <v>0.541666666666667</v>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C35" s="3">
+        <v>0.54166666666666696</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>54</v>
@@ -1104,17 +1069,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="3" t="n">
-        <v>0.597222222222222</v>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C36" s="3">
+        <v>0.59722222222222199</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="3" t="n">
-        <v>0.611111111111111</v>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C37" s="3">
+        <v>0.61111111111111105</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>54</v>
@@ -1123,9 +1088,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="3" t="n">
-        <v>0.697916666666667</v>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C38" s="3">
+        <v>0.69791666666666696</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>55</v>
@@ -1134,14 +1099,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="3">
         <v>0.375</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -1154,56 +1119,56 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="3" t="n">
-        <v>0.430555555555556</v>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C40" s="3">
+        <v>0.43055555555555602</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="3" t="n">
-        <v>0.444444444444444</v>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C41" s="3">
+        <v>0.44444444444444398</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="3" t="n">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C42" s="3">
         <v>0.5</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="3" t="n">
-        <v>0.541666666666667</v>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C43" s="3">
+        <v>0.54166666666666696</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="3" t="n">
-        <v>0.597222222222222</v>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C44" s="3">
+        <v>0.59722222222222199</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="3" t="n">
-        <v>0.611111111111111</v>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C45" s="3">
+        <v>0.61111111111111105</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="3" t="n">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C46" s="3">
         <v>0.65625</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1214,13 +1179,8 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update schedule for DDLS course
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlarsson/git/workshop-reproducible-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C74F37-60FD-714B-B232-4E36D4D64528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C55C3CD-B4A6-0146-AC10-5D83A171F0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26420" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="26420" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$J$30</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -93,9 +93,6 @@
     <t>link_room</t>
   </si>
   <si>
-    <t>25/11/2024</t>
-  </si>
-  <si>
     <t>Stockholm</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Wrap-up day 1</t>
   </si>
   <si>
-    <t>26/11/2024</t>
-  </si>
-  <si>
     <t>Organise your analyses using workflow managers: Snakemake</t>
   </si>
   <si>
@@ -180,9 +174,6 @@
     <t>Course dinner</t>
   </si>
   <si>
-    <t>27/11/2024</t>
-  </si>
-  <si>
     <t>… continued: Nextflow</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>Wrap-up day 3</t>
   </si>
   <si>
-    <t>28/11/2024</t>
-  </si>
-  <si>
     <t>… continued: Jupyter</t>
   </si>
   <si>
@@ -231,9 +219,6 @@
     <t>Wrap-up day 4</t>
   </si>
   <si>
-    <t>29/11/2024</t>
-  </si>
-  <si>
     <t>Putting it all together</t>
   </si>
   <si>
@@ -247,6 +232,21 @@
   </si>
   <si>
     <t>pages/introduction.html</t>
+  </si>
+  <si>
+    <t>06/10/2025</t>
+  </si>
+  <si>
+    <t>07/10/2025</t>
+  </si>
+  <si>
+    <t>08/10/2025</t>
+  </si>
+  <si>
+    <t>09/10/2025</t>
+  </si>
+  <si>
+    <t>10/10/2025</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,16 +649,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -666,16 +666,16 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -684,7 +684,7 @@
         <v>0.43402777777777801</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -692,13 +692,13 @@
         <v>0.44444444444444398</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -706,16 +706,16 @@
         <v>0.46527777777777801</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -724,7 +724,7 @@
         <v>0.5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -732,10 +732,10 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -743,7 +743,7 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -751,16 +751,16 @@
         <v>0.625</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -768,33 +768,33 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>0.375</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -803,7 +803,7 @@
         <v>0.43055555555555602</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -811,10 +811,10 @@
         <v>0.44444444444444398</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -822,7 +822,7 @@
         <v>0.5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -831,10 +831,10 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -842,7 +842,7 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -853,16 +853,16 @@
         <v>0.625</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -870,10 +870,10 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I19" s="4"/>
     </row>
@@ -882,25 +882,25 @@
         <v>0.75</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3">
         <v>0.375</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -908,7 +908,7 @@
         <v>0.43055555555555602</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I22" s="4"/>
     </row>
@@ -917,10 +917,10 @@
         <v>0.44444444444444398</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -928,7 +928,7 @@
         <v>0.5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="4"/>
     </row>
@@ -937,16 +937,16 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -962,10 +962,10 @@
         <v>0.61805555555555602</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -973,16 +973,16 @@
         <v>0.63888888888888895</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -990,27 +990,27 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="3">
         <v>0.375</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I30" s="4"/>
     </row>
@@ -1019,16 +1019,16 @@
         <v>0.40625</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1036,7 +1036,7 @@
         <v>0.4375</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1044,10 +1044,10 @@
         <v>0.45138888888888901</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1055,7 +1055,7 @@
         <v>0.5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1063,10 +1063,10 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1074,7 +1074,7 @@
         <v>0.59722222222222199</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1082,10 +1082,10 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1093,30 +1093,30 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39" s="3">
         <v>0.375</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1124,7 +1124,7 @@
         <v>0.43055555555555602</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1132,7 +1132,7 @@
         <v>0.44444444444444398</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1140,7 +1140,7 @@
         <v>0.5</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1148,7 +1148,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1156,7 +1156,7 @@
         <v>0.59722222222222199</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1172,10 +1172,10 @@
         <v>0.65625</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix link to conda tutorial
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlarsson/git/workshop-reproducible-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5404F307-133E-A84F-89E3-4FFF31749D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534146C4-BA58-C145-AF90-65B9E433EE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="17060" windowHeight="21260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>date</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Stephan Nylinder</t>
+  </si>
+  <si>
+    <t>pages/conda.html</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,7 +732,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add documentation to schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlarsson/git/workshop-reproducible-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6222527B-4325-594B-9ACB-B0931567FD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F0ACF6-3540-B142-9D17-3ED7FBDA6620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="680" windowWidth="30200" windowHeight="21660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>date</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>Lokesh Mano</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>lectures/documentation/documentation.html</t>
+  </si>
+  <si>
+    <t>pages/documentation.html</t>
   </si>
 </sst>
 </file>
@@ -325,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -333,6 +342,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -595,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1088,75 +1098,92 @@
       <c r="B38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="7">
         <v>0.375</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C39" s="3">
-        <v>0.43055555555555602</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>11</v>
+        <v>43</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C40" s="3">
-        <v>0.44444444444444398</v>
+        <v>0.43055555555555602</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C41" s="3">
-        <v>0.5</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C42" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.5</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C43" s="3">
-        <v>0.59722222222222199</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C44" s="3">
-        <v>0.61111111111111105</v>
+        <v>0.59722222222222199</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C45" s="3">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C46" s="3">
         <v>0.65625</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change schedule with new session order
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,18 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikfasterius/teaching/workshop-reproducible-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F0ACF6-3540-B142-9D17-3ED7FBDA6620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454BCD90-20A2-174E-AC14-097EE32B81F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="680" windowWidth="30200" windowHeight="21660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$J$29</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$J$31</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -61,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
   <si>
     <t>date</t>
   </si>
@@ -96,12 +106,30 @@
     <t>Stockholm</t>
   </si>
   <si>
+    <t>Setting up and troubleshooting installations</t>
+  </si>
+  <si>
+    <t>Introduction to Reproducible Research</t>
+  </si>
+  <si>
+    <t>Erik Fasterius</t>
+  </si>
+  <si>
+    <t>lectures/introduction/introduction.html</t>
+  </si>
+  <si>
     <t>Break</t>
   </si>
   <si>
+    <t>Data management and project organisation</t>
+  </si>
+  <si>
     <t>John Sundh</t>
   </si>
   <si>
+    <t>lectures/data-management/data-management.html</t>
+  </si>
+  <si>
     <t>Version tracking and distributing your code</t>
   </si>
   <si>
@@ -114,12 +142,18 @@
     <t>Lunch</t>
   </si>
   <si>
+    <t>… continued: Git</t>
+  </si>
+  <si>
     <t>Controlling your environment with Conda</t>
   </si>
   <si>
     <t>lectures/conda/conda.html</t>
   </si>
   <si>
+    <t>pages/conda.html</t>
+  </si>
+  <si>
     <t>Wrap-up day 1</t>
   </si>
   <si>
@@ -147,6 +181,9 @@
     <t>Wrap-up day 2</t>
   </si>
   <si>
+    <t>Course dinner</t>
+  </si>
+  <si>
     <t>… continued: Nextflow</t>
   </si>
   <si>
@@ -204,43 +241,7 @@
     <t>Final wrap-up and end of the course</t>
   </si>
   <si>
-    <t>06/10/2025</t>
-  </si>
-  <si>
-    <t>07/10/2025</t>
-  </si>
-  <si>
-    <t>08/10/2025</t>
-  </si>
-  <si>
-    <t>09/10/2025</t>
-  </si>
-  <si>
-    <t>10/10/2025</t>
-  </si>
-  <si>
-    <t>Course dinner @ Haga Bottega, Eugeniavägen 6</t>
-  </si>
-  <si>
-    <t>Project organisation showcases</t>
-  </si>
-  <si>
-    <t>Elin Kronander</t>
-  </si>
-  <si>
-    <t>Introduction</t>
-  </si>
-  <si>
-    <t>Metadata</t>
-  </si>
-  <si>
-    <t>Stephan Nylinder</t>
-  </si>
-  <si>
-    <t>pages/conda.html</t>
-  </si>
-  <si>
-    <t>Lokesh Mano</t>
+    <t>pages/introduction.html</t>
   </si>
   <si>
     <t>Documentation</t>
@@ -250,6 +251,21 @@
   </si>
   <si>
     <t>pages/documentation.html</t>
+  </si>
+  <si>
+    <t>20/04/2026</t>
+  </si>
+  <si>
+    <t>21/04/2026</t>
+  </si>
+  <si>
+    <t>22/04/2026</t>
+  </si>
+  <si>
+    <t>23/04/2026</t>
+  </si>
+  <si>
+    <t>24/04/2026</t>
   </si>
 </sst>
 </file>
@@ -259,7 +275,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -306,12 +322,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -334,15 +344,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -605,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +628,7 @@
     <col min="5" max="5" width="30" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="45.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="10.6640625" style="1"/>
@@ -660,7 +668,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -669,522 +677,543 @@
         <v>0.375</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
       <c r="C3" s="3">
-        <v>0.38541666666666669</v>
+        <v>0.41666666666666702</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
-        <v>0.41666666666666702</v>
+        <v>0.43402777777777801</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="4"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
-        <v>0.43055555555555558</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="3">
-        <v>0.5</v>
+        <v>0.46527777777777801</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="4"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8" s="3">
-        <v>0.61111111111111116</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
-        <v>0.625</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
-        <v>0.69791666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="3">
+        <v>0.69791666666666696</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="3">
-        <v>0.43055555555555602</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="H12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="3">
-        <v>0.44444444444444398</v>
+        <v>0.43055555555555602</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" s="3">
-        <v>0.5</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C16" s="3">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="C16" s="3">
-        <v>0.61111111111111105</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C17" s="3">
         <v>0.625</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C18" s="3">
-        <v>0.69791666666666696</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C19" s="3">
-        <v>0.72916666666666663</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C21" s="3">
         <v>0.375</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C21" s="3">
-        <v>0.43055555555555602</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
       <c r="C22" s="3">
-        <v>0.44444444444444398</v>
+        <v>0.40625</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
-        <v>0.5</v>
+        <v>0.43055555555555602</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C24" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C25" s="3">
-        <v>0.60416666666666696</v>
+        <v>0.5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C26" s="3">
-        <v>0.61805555555555602</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C27" s="3">
-        <v>0.63888888888888895</v>
+        <v>0.5625</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C28" s="3">
-        <v>0.69791666666666696</v>
+        <v>0.60416666666666696</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C29" s="3">
-        <v>0.375</v>
+        <v>0.61805555555555602</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="4"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C30" s="3">
-        <v>0.40625</v>
+        <v>0.69791666666666696</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C31" s="3">
-        <v>0.4375</v>
+        <v>0.375</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C32" s="3">
-        <v>0.45138888888888901</v>
+        <v>0.4375</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C33" s="3">
-        <v>0.5</v>
+        <v>0.45138888888888901</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C34" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C35" s="3">
-        <v>0.59722222222222199</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C36" s="3">
-        <v>0.61111111111111105</v>
+        <v>0.59722222222222199</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C37" s="3">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C38" s="3">
         <v>0.69791666666666696</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="E38" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C39" s="3">
         <v>0.375</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C39" s="3">
-        <v>0.38541666666666669</v>
-      </c>
       <c r="D39" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C40" s="3">
-        <v>0.43055555555555602</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C41" s="3">
-        <v>0.44444444444444398</v>
+        <v>0.43055555555555602</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C42" s="3">
-        <v>0.5</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C43" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.5</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C44" s="3">
-        <v>0.59722222222222199</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C45" s="3">
-        <v>0.61111111111111105</v>
+        <v>0.59722222222222199</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C46" s="3">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C47" s="3">
         <v>0.65625</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>12</v>
+      <c r="D47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>